<commit_message>
Actualización: incluye tiempo de espera y ajustes de inputs
</commit_message>
<xml_diff>
--- a/Boater_excel.xlsx
+++ b/Boater_excel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrestorres/Documents/Boater/Calculo costo viaje/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979B2C85-6ADA-4A4F-8394-40F676BCB6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Motor fuera de borda</t>
   </si>
@@ -46,12 +47,21 @@
   <si>
     <t>coeficiente Asientos</t>
   </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>espera (€)</t>
+  </si>
+  <si>
+    <t>costo hora de espera/km</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,8 +69,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +97,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -92,13 +116,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,19 +401,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AZ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -545,7 +571,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -703,7 +729,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -861,7 +887,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1019,7 +1045,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1105,7 +1131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1277,7 +1303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1363,17 +1389,105 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3">
+        <v>13</v>
+      </c>
+      <c r="F18" s="3">
+        <v>14</v>
+      </c>
+      <c r="G18" s="3">
+        <v>15</v>
+      </c>
+      <c r="H18" s="3">
+        <v>16</v>
+      </c>
+      <c r="I18" s="3">
+        <v>17</v>
+      </c>
+      <c r="J18" s="3">
+        <v>18</v>
+      </c>
+      <c r="K18" s="3">
+        <v>19</v>
+      </c>
+      <c r="L18" s="3">
+        <v>20</v>
+      </c>
+      <c r="M18" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4">
+        <v>14</v>
+      </c>
+      <c r="D19" s="4">
+        <v>14</v>
+      </c>
+      <c r="E19" s="4">
+        <v>13</v>
+      </c>
+      <c r="F19" s="4">
+        <v>13</v>
+      </c>
+      <c r="G19" s="4">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4">
+        <v>12</v>
+      </c>
+      <c r="I19" s="4">
+        <v>11</v>
+      </c>
+      <c r="J19" s="4">
+        <v>11</v>
+      </c>
+      <c r="K19" s="4">
+        <v>10</v>
+      </c>
+      <c r="L19" s="4">
+        <v>10</v>
+      </c>
+      <c r="M19" s="4">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nuevo Excel corregido manualmente
</commit_message>
<xml_diff>
--- a/Boater_excel.xlsx
+++ b/Boater_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrestorres/Documents/Boater/Calculo costo viaje/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCB9893-6A80-5546-BAEA-11C74DC28097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2020CC9-706F-994A-B246-C98E41B7495B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14900" yWindow="-19380" windowWidth="76800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -116,12 +116,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +406,7 @@
   <dimension ref="A1:AZ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1391,103 +1392,105 @@
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3">
+        <v>13</v>
+      </c>
+      <c r="F13" s="3">
+        <v>14</v>
+      </c>
+      <c r="G13" s="3">
+        <v>15</v>
+      </c>
+      <c r="H13" s="3">
+        <v>16</v>
+      </c>
+      <c r="I13" s="3">
+        <v>17</v>
+      </c>
+      <c r="J13" s="3">
+        <v>18</v>
+      </c>
+      <c r="K13" s="3">
+        <v>19</v>
+      </c>
+      <c r="L13" s="3">
+        <v>20</v>
+      </c>
+      <c r="M13" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4">
+        <v>14</v>
+      </c>
+      <c r="E14" s="4">
+        <v>13</v>
+      </c>
+      <c r="F14" s="4">
+        <v>13</v>
+      </c>
+      <c r="G14" s="4">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4">
+        <v>12</v>
+      </c>
+      <c r="I14" s="4">
+        <v>11</v>
+      </c>
+      <c r="J14" s="4">
+        <v>11</v>
+      </c>
+      <c r="K14" s="4">
+        <v>10</v>
+      </c>
+      <c r="L14" s="4">
+        <v>10</v>
+      </c>
+      <c r="M14" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:52" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B17" s="1"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B18" s="2"/>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3">
-        <v>10</v>
-      </c>
-      <c r="C18" s="3">
-        <v>11</v>
-      </c>
-      <c r="D18" s="3">
-        <v>12</v>
-      </c>
-      <c r="E18" s="3">
-        <v>13</v>
-      </c>
-      <c r="F18" s="3">
-        <v>14</v>
-      </c>
-      <c r="G18" s="3">
-        <v>15</v>
-      </c>
-      <c r="H18" s="3">
-        <v>16</v>
-      </c>
-      <c r="I18" s="3">
-        <v>17</v>
-      </c>
-      <c r="J18" s="3">
-        <v>18</v>
-      </c>
-      <c r="K18" s="3">
-        <v>19</v>
-      </c>
-      <c r="L18" s="3">
-        <v>20</v>
-      </c>
-      <c r="M18" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="4">
-        <v>15</v>
-      </c>
-      <c r="C19" s="4">
-        <v>14</v>
-      </c>
-      <c r="D19" s="4">
-        <v>14</v>
-      </c>
-      <c r="E19" s="4">
-        <v>13</v>
-      </c>
-      <c r="F19" s="4">
-        <v>13</v>
-      </c>
-      <c r="G19" s="4">
-        <v>12</v>
-      </c>
-      <c r="H19" s="4">
-        <v>12</v>
-      </c>
-      <c r="I19" s="4">
-        <v>11</v>
-      </c>
-      <c r="J19" s="4">
-        <v>11</v>
-      </c>
-      <c r="K19" s="4">
-        <v>10</v>
-      </c>
-      <c r="L19" s="4">
-        <v>10</v>
-      </c>
-      <c r="M19" s="4">
-        <v>10</v>
-      </c>
+      <c r="B19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Boater Excel corregido con etiquetas válidas y formato final
</commit_message>
<xml_diff>
--- a/Boater_excel.xlsx
+++ b/Boater_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrestorres/Documents/Boater/Calculo costo viaje/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2020CC9-706F-994A-B246-C98E41B7495B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54E2F80F-6980-7549-95E6-3A4C7DB3E902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14900" yWindow="-19380" windowWidth="76800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23200" yWindow="-21100" windowWidth="76800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -116,13 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1472,8 +1471,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:52" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:52" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:52" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:52" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>

</xml_diff>